<commit_message>
Objectos del DOM y el BOM
</commit_message>
<xml_diff>
--- a/Semana4/Dia1/TAREA.xlsx
+++ b/Semana4/Dia1/TAREA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Garnica\Documents\CodiGo3\CodiGo3\Semana4\Dia1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5289D47E-4F8F-4F66-B94F-FC70EE357E23}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD8069D-9886-496F-8784-D929A86D730A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{025319D3-21B8-4B5A-8447-40CB5B197B3F}"/>
   </bookViews>
@@ -144,19 +144,19 @@
     <t>verInfoDeTemporada</t>
   </si>
   <si>
-    <t>100 =&gt; A soles en base al consumo</t>
-  </si>
-  <si>
-    <t>80 =&gt; B soles en base al consumo</t>
-  </si>
-  <si>
-    <t>70 =&gt; C soles en base al consumo</t>
-  </si>
-  <si>
     <t>Si la propiedad "alquilado" es true, mostrar mensaje de error por que la serie está alquilada, si es FALSE, cambiar el valor de la variable a TRUE y mostrar mensaje de "alquilado"</t>
   </si>
   <si>
     <t>Recibirá un numero de la temporada, y se mostrará la descripción de la temporada</t>
+  </si>
+  <si>
+    <t>100 =&gt; A  en base al consumo</t>
+  </si>
+  <si>
+    <t>80 =&gt; B  en base al consumo</t>
+  </si>
+  <si>
+    <t>70 =&gt; C  en base al consumo</t>
   </si>
 </sst>
 </file>
@@ -320,15 +320,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -339,6 +330,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369A4A1C-D6AC-4FE2-B32D-664D1E9CEBF6}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,11 +826,11 @@
       <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>13</v>
@@ -842,9 +842,9 @@
       <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>13</v>
@@ -856,39 +856,39 @@
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -896,7 +896,7 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="3" t="s">
         <v>27</v>
       </c>
@@ -948,7 +948,7 @@
         <v>37</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>18</v>
@@ -964,7 +964,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>18</v>
@@ -1015,44 +1015,44 @@
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>